<commit_message>
course controller and question upload
</commit_message>
<xml_diff>
--- a/onlineexam/test_excel/test_write_a.xlsx
+++ b/onlineexam/test_excel/test_write_a.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="12648" windowWidth="22260" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -59,6 +59,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -93,19 +94,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -122,10 +123,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -160,7 +161,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -195,7 +196,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -289,21 +290,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -320,7 +321,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -372,23 +373,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C5" sqref="A3:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.5546875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -409,7 +410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -420,7 +421,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -436,7 +437,7 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>